<commit_message>
Update formato.xlsx with new data and formatting improvements
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e039d0c270e9facf/Desktop/Developer/UANL---LABORATORIO-DE-ALIMENTOS-MEDICAMENTOS-Y-TOXICOLOGIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{47FAC42F-AC07-43D6-8172-01CEADEBF0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{096DE1EE-21D0-4E14-A1A4-462374911631}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{47FAC42F-AC07-43D6-8172-01CEADEBF0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE20E0D3-69CA-4567-8916-9B0C917BE083}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CB8A4CE-E91B-448F-9BE6-E546BA7C8907}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1CB8A4CE-E91B-448F-9BE6-E546BA7C8907}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>UANL FACULTAD DE CIENCIAS QUÍMICAS</t>
-  </si>
-  <si>
-    <t>Laboratorio de Alimentos, Medicamentos y Toxicología</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>1. TABLA DE INFORMACIÓN NUTRIMENTAL (DECLARACIÓN NUTRIMENTAL)</t>
   </si>
@@ -74,9 +68,6 @@
     <t>ESPECIFICACIONES GENERALES DE ETIQUETADO PARA ALIMENTOS Y BEBIDAS NO ALCOHÓLICAS PREENVASADOS NOM-051-SCFI/SSA1-2010.</t>
   </si>
   <si>
-    <t>Tel. 8188 2940 00 Ext. 6332, Directo: 8183 5298 91 | e-mail: laboratorio.alimentos@hotmail.com</t>
-  </si>
-  <si>
     <t>Declaración Nutrimental</t>
   </si>
   <si>
@@ -90,12 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">          Azúcares añadidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNIVERSIDAD AUTÓNOMA DE NUEVO LEÓN </t>
-  </si>
-  <si>
-    <t>Av Universidad s/n, Cd. Universitaria, C.P 66455, San Nicolás de los Garza, N.L.</t>
   </si>
   <si>
     <t xml:space="preserve">Tamaño de la porción: </t>
@@ -365,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -398,6 +383,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,42 +441,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,283 +465,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>516095</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>588644</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>131445</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Notas Educativas">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC43186-AA06-DC4F-D77F-4702D66C4FD2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="516095" y="167640"/>
-          <a:ext cx="685959" cy="888365"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>4128</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>167005</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Connector 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA7BA78-5E56-8643-0EDC-718D9D9DB312}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1223328" y="187960"/>
-          <a:ext cx="8572" cy="531495"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>157002</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>39053</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>94806</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>58103</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="Facultad De Ciencias Quimicas logo, Vector Logo of Facultad De Ciencias ...">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{035CFF72-40D6-C4F2-ED61-2B525BEACA46}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1376202" y="223203"/>
-          <a:ext cx="556929" cy="567690"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>433400</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>113983</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>495934</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>473394</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="Servicios en línea - Universidad Autónoma de Nuevo León">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{434931BB-DEC6-80D2-3523-B00A86E0DC7D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2266963" y="6590983"/>
-          <a:ext cx="673721" cy="538163"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>94310</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>67628</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>78115</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>474029</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D4453BC-E1F5-8929-1637-1D29A4110D45}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3150248" y="6544628"/>
-          <a:ext cx="928367" cy="581343"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>428624</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -766,7 +472,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
+      <xdr:colOff>358775</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>154940</xdr:rowOff>
     </xdr:to>
@@ -784,7 +490,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -827,7 +533,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
+      <xdr:colOff>403225</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>153035</xdr:rowOff>
     </xdr:to>
@@ -845,7 +551,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -906,7 +612,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -949,7 +655,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>198439</xdr:colOff>
+      <xdr:colOff>209869</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>135572</xdr:rowOff>
     </xdr:to>
@@ -967,7 +673,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1010,9 +716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>27939</xdr:colOff>
+      <xdr:colOff>22224</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>140969</xdr:rowOff>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1028,7 +734,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1044,6 +750,128 @@
         <a:xfrm>
           <a:off x="8556625" y="1966595"/>
           <a:ext cx="1210627" cy="1373187"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7619</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B3A08D5-A483-DDAB-542B-14F9D484D135}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="13298" b="19367"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="7619"/>
+          <a:ext cx="6330315" cy="920115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>237027</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6203F574-3C04-A485-6D5F-473451DC571C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="6686550"/>
+          <a:ext cx="6580677" cy="1358265"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1388,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677BF1A9-BE92-4F6B-8063-3CDF98601680}">
   <dimension ref="A4:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A42" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1403,32 +1231,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -1455,43 +1279,38 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="B8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
+      <c r="B10" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="B12" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1506,17 +1325,17 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="B15" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="38"/>
+      <c r="B15" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
@@ -1524,10 +1343,10 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="39"/>
+      <c r="C17" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="30"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1537,10 +1356,10 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="39"/>
+      <c r="C18" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="30"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -1550,11 +1369,11 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="14"/>
@@ -1566,23 +1385,23 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="35"/>
-      <c r="H20" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="29"/>
+      <c r="F20" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="26"/>
+      <c r="H20" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="40"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
-      <c r="C21" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
+      <c r="C21" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="18"/>
       <c r="G21" s="19"/>
       <c r="H21" s="16"/>
@@ -1591,11 +1410,11 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
-      <c r="C22" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
+      <c r="C22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
       <c r="H22" s="16"/>
@@ -1604,11 +1423,11 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
-      <c r="C23" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
+      <c r="C23" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
       <c r="H23" s="16"/>
@@ -1617,11 +1436,11 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
-      <c r="C24" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
+      <c r="C24" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
       <c r="H24" s="18"/>
@@ -1629,11 +1448,11 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
-      <c r="C25" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="C25" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
       <c r="F25" s="18"/>
       <c r="G25" s="19"/>
       <c r="H25" s="18"/>
@@ -1641,11 +1460,11 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
-      <c r="C26" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
+      <c r="C26" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="16"/>
       <c r="G26" s="17"/>
       <c r="H26" s="16"/>
@@ -1654,10 +1473,10 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
-      <c r="C27" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="30"/>
+      <c r="C27" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="41"/>
       <c r="F27" s="18"/>
       <c r="G27" s="19"/>
       <c r="H27" s="18"/>
@@ -1666,7 +1485,7 @@
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
       <c r="C28" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D28" s="13"/>
       <c r="F28" s="18"/>
@@ -1676,10 +1495,10 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
-      <c r="C29" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="31"/>
+      <c r="C29" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="23"/>
       <c r="E29" s="10"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
@@ -1689,10 +1508,10 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
-      <c r="C30" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="32"/>
+      <c r="C30" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="24"/>
       <c r="E30" s="10"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
@@ -1712,67 +1531,54 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="2:10" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="28"/>
+      <c r="B32" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="39"/>
     </row>
     <row r="36" spans="2:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:E19"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B37:J37"/>
     <mergeCell ref="B38:J38"/>
@@ -1789,6 +1595,13 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new images for "sodio" and "trans" to the Sellos directory; create an empty info2.txt file.
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e039d0c270e9facf/Desktop/Developer/UANL---LABORATORIO-DE-ALIMENTOS-MEDICAMENTOS-Y-TOXICOLOGIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{47FAC42F-AC07-43D6-8172-01CEADEBF0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE20E0D3-69CA-4567-8916-9B0C917BE083}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{47FAC42F-AC07-43D6-8172-01CEADEBF0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386991D7-84E1-4C50-B832-FF34AF9BA7DD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1CB8A4CE-E91B-448F-9BE6-E546BA7C8907}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CB8A4CE-E91B-448F-9BE6-E546BA7C8907}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,12 +384,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -410,39 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,311 +463,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>59690</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>358775</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>154940</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="Nuevo etiquetado para alimentos en México">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40C8EC3B-6057-25C1-D976-0452FC643E27}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect r="80050"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6500812" y="607378"/>
-          <a:ext cx="1143001" cy="1373187"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>559435</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>403225</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>153035</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="Nuevo etiquetado para alimentos en México">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDA55F14-4090-5801-3E40-B4B49FF9A0A1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="19744" r="61413"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7853998" y="601663"/>
-          <a:ext cx="1075690" cy="1376997"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>147003</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>39688</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>20003</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>131128</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="Nuevo etiquetado para alimentos en México">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CFA252A-7B50-33F5-926E-FDDBD3234EC6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="39252" r="41673"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9275128" y="587376"/>
-          <a:ext cx="1095375" cy="1369377"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>55562</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>209869</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>135572</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="Nuevo etiquetado para alimentos en México">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88D462EC-71F0-2B6F-59C6-1656DFED87BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="58307" r="21387"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10604500" y="603250"/>
-          <a:ext cx="1166814" cy="1357947"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>39687</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>22224</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="Nuevo etiquetado para alimentos en México">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3271705B-2139-031C-4BC3-B00E08053526}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="78969"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8556625" y="1966595"/>
-          <a:ext cx="1210627" cy="1373187"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -795,7 +490,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -838,7 +533,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>237027</xdr:colOff>
+      <xdr:colOff>248457</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
@@ -856,7 +551,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1214,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677BF1A9-BE92-4F6B-8063-3CDF98601680}">
-  <dimension ref="A4:J39"/>
+  <dimension ref="A4:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A42" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C42" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1228,31 +923,34 @@
     <col min="8" max="8" width="8.88671875" customWidth="1"/>
     <col min="9" max="9" width="3.44140625" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="15" max="15" width="17.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -1292,25 +990,25 @@
       <c r="J8" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1325,17 +1023,17 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="40"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
@@ -1343,10 +1041,10 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="30"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1356,10 +1054,10 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -1369,11 +1067,11 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="14"/>
@@ -1385,23 +1083,23 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="40" t="s">
+      <c r="G20" s="37"/>
+      <c r="H20" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="40"/>
+      <c r="I20" s="31"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
       <c r="F21" s="18"/>
       <c r="G21" s="19"/>
       <c r="H21" s="16"/>
@@ -1410,11 +1108,11 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
       <c r="H22" s="16"/>
@@ -1423,11 +1121,11 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
       <c r="H23" s="16"/>
@@ -1436,11 +1134,11 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
       <c r="H24" s="18"/>
@@ -1448,11 +1146,11 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
       <c r="F25" s="18"/>
       <c r="G25" s="19"/>
       <c r="H25" s="18"/>
@@ -1460,11 +1158,11 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
       <c r="F26" s="16"/>
       <c r="G26" s="17"/>
       <c r="H26" s="16"/>
@@ -1473,10 +1171,10 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="41"/>
+      <c r="D27" s="32"/>
       <c r="F27" s="18"/>
       <c r="G27" s="19"/>
       <c r="H27" s="18"/>
@@ -1495,10 +1193,10 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="23"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="10"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
@@ -1508,10 +1206,10 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="24"/>
+      <c r="D30" s="34"/>
       <c r="E30" s="10"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
@@ -1531,54 +1229,63 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="2:10" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="39"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="30"/>
     </row>
     <row r="36" spans="2:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-    </row>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+    </row>
+    <row r="44" spans="2:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:E19"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B37:J37"/>
     <mergeCell ref="B38:J38"/>
@@ -1595,13 +1302,6 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add NutrimentalExporter class for exporting nutritional data to Excel and PDF
- Implemented methods for filling Excel templates with nutritional data.
- Added functionality to generate PDF files from Excel using COM.
- Included image handling for warning seals based on nutritional content.
- Integrated user input validation and error handling for file operations.
- Created methods for saving data to a database with detailed descriptions.
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e039d0c270e9facf/Desktop/Developer/UANL---LABORATORIO-DE-ALIMENTOS-MEDICAMENTOS-Y-TOXICOLOGIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{47FAC42F-AC07-43D6-8172-01CEADEBF0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386991D7-84E1-4C50-B832-FF34AF9BA7DD}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{47FAC42F-AC07-43D6-8172-01CEADEBF0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{916F2CCF-DC7F-4EEF-8AE2-D0D5A0F8E5EE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CB8A4CE-E91B-448F-9BE6-E546BA7C8907}"/>
   </bookViews>
@@ -384,6 +384,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -436,12 +438,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -468,13 +464,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
+      <xdr:rowOff>7618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:colOff>624840</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>94601</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -504,8 +500,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="7619"/>
-          <a:ext cx="6330315" cy="920115"/>
+          <a:off x="0" y="7618"/>
+          <a:ext cx="6362700" cy="1001383"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -533,7 +529,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>248457</xdr:colOff>
+      <xdr:colOff>225597</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
@@ -911,13 +907,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677BF1A9-BE92-4F6B-8063-3CDF98601680}">
   <dimension ref="A4:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C42" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="4.88671875" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" customWidth="1"/>
@@ -929,28 +926,28 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -990,25 +987,25 @@
       <c r="J8" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1023,17 +1020,17 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="42"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
@@ -1041,12 +1038,12 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="41"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -1054,12 +1051,11 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="11"/>
       <c r="I18" s="10"/>
@@ -1067,11 +1063,11 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="14"/>
@@ -1083,23 +1079,23 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="31" t="s">
+      <c r="G20" s="39"/>
+      <c r="H20" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="31"/>
+      <c r="I20" s="33"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="18"/>
       <c r="G21" s="19"/>
       <c r="H21" s="16"/>
@@ -1108,11 +1104,11 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
       <c r="H22" s="16"/>
@@ -1121,11 +1117,11 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
       <c r="H23" s="16"/>
@@ -1134,11 +1130,11 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
       <c r="H24" s="18"/>
@@ -1146,11 +1142,11 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="18"/>
       <c r="G25" s="19"/>
       <c r="H25" s="18"/>
@@ -1158,11 +1154,11 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="16"/>
       <c r="G26" s="17"/>
       <c r="H26" s="16"/>
@@ -1171,10 +1167,10 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="34"/>
       <c r="F27" s="18"/>
       <c r="G27" s="19"/>
       <c r="H27" s="18"/>
@@ -1193,10 +1189,10 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="33"/>
+      <c r="D29" s="35"/>
       <c r="E29" s="10"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
@@ -1206,10 +1202,10 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="34"/>
+      <c r="D30" s="36"/>
       <c r="E30" s="10"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
@@ -1229,63 +1225,60 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="2:10" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="32"/>
     </row>
     <row r="36" spans="2:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
     </row>
     <row r="44" spans="2:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="2:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="20">
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="B15:J15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:E19"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B37:J37"/>
     <mergeCell ref="B38:J38"/>

</xml_diff>